<commit_message>
Updates to Measurment Chain + Current Calc
</commit_message>
<xml_diff>
--- a/2.2 Measurement Chain/signal-conditioning_calc.xlsx
+++ b/2.2 Measurement Chain/signal-conditioning_calc.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\HSRW\Semester 5\Group Project\Group-Project_WS2526\2.2 Measurement Chain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CB80C5-46FE-470A-854F-B5B9B25310EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F1DA83-CF69-492B-B476-57BE5E9724A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INA + VGA" sheetId="2" r:id="rId1"/>
-    <sheet name="nur INA" sheetId="1" r:id="rId2"/>
+    <sheet name="Battery Estimate" sheetId="4" r:id="rId2"/>
+    <sheet name="Load Cell Current" sheetId="3" r:id="rId3"/>
+    <sheet name="nur INA" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Load Cell [kgf]</t>
   </si>
@@ -97,6 +99,60 @@
   </si>
   <si>
     <t>Actual VGA Gain</t>
+  </si>
+  <si>
+    <t>I @5V [mA]</t>
+  </si>
+  <si>
+    <t>I @10V [mA]</t>
+  </si>
+  <si>
+    <t>Bridge Resistance [Ohm]</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>I_typ [mA]</t>
+  </si>
+  <si>
+    <t>I_max [mA]</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Load Cell</t>
+  </si>
+  <si>
+    <t>LDO</t>
+  </si>
+  <si>
+    <t>INA</t>
+  </si>
+  <si>
+    <t>OPAMP</t>
+  </si>
+  <si>
+    <t>Digi Poti</t>
+  </si>
+  <si>
+    <t>Estimate Typ [h]</t>
+  </si>
+  <si>
+    <t>Estimate Min [h]</t>
+  </si>
+  <si>
+    <t>DS ADC</t>
+  </si>
+  <si>
+    <t>Total I_typ</t>
+  </si>
+  <si>
+    <t>Total I_max</t>
+  </si>
+  <si>
+    <t>VREF</t>
   </si>
 </sst>
 </file>
@@ -106,7 +162,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
-    <numFmt numFmtId="167" formatCode="0.000%"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -145,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -154,7 +210,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6EE15B-76DB-48AD-8A28-EECC0E4E87EC}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,6 +852,296 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D73221-315D-4403-8AB8-0BEE10775D1A}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>14.28</v>
+      </c>
+      <c r="C2">
+        <v>28.57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2">
+        <f>SUM(B2:B100)</f>
+        <v>22.256</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2">
+        <f>SUM(B3:B100)</f>
+        <v>7.976</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3">
+        <f>SUM(C2:C100)</f>
+        <v>38.121999999999993</v>
+      </c>
+      <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3">
+        <f>SUM(C3:C100)</f>
+        <v>9.5520000000000014</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>0.45</v>
+      </c>
+      <c r="C5">
+        <v>0.51</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5">
+        <f>H4/H3</f>
+        <v>131.15786160222447</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>1E-3</v>
+      </c>
+      <c r="C6">
+        <v>2E-3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6">
+        <f>H4/H2</f>
+        <v>224.65851905104242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8">
+        <v>0.38</v>
+      </c>
+      <c r="C8">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A0FFB42-0A8F-436F-9B31-E7D1096635CF}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="B2">
+        <v>350</v>
+      </c>
+      <c r="C2">
+        <f>5/$B2 * 1000</f>
+        <v>14.285714285714285</v>
+      </c>
+      <c r="D2">
+        <f>10/$B2 * 1000</f>
+        <v>28.571428571428569</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>350</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C7" si="0">5/$B3 * 1000</f>
+        <v>14.285714285714285</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D7" si="1">10/$B3 * 1000</f>
+        <v>28.571428571428569</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>175</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>28.571428571428569</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>57.142857142857139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>350</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>14.285714285714285</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>28.571428571428569</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>250</v>
+      </c>
+      <c r="B6">
+        <v>175</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>28.571428571428569</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>57.142857142857139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>3000</v>
+      </c>
+      <c r="B7">
+        <v>175</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>28.571428571428569</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>57.142857142857139</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
+    <sortCondition ref="A1:A7"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>

</xml_diff>

<commit_message>
Sig fig in Excel
</commit_message>
<xml_diff>
--- a/2.2 Measurement Chain/signal-conditioning_calc.xlsx
+++ b/2.2 Measurement Chain/signal-conditioning_calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\HSRW\Semester 5\Group Project\Group-Project_WS2526\2.2 Measurement Chain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EE7790-F564-401B-B7AD-63873A008677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D3FBAD-7CB4-48D0-A850-2C9F887F7C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INA + VGA" sheetId="2" r:id="rId1"/>
@@ -251,7 +251,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -263,6 +263,10 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -547,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6EE15B-76DB-48AD-8A28-EECC0E4E87EC}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,275 +604,279 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>3000</v>
+        <v>0.15</v>
       </c>
       <c r="B2" s="1">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <f>B2*5</f>
-        <v>14</v>
-      </c>
-      <c r="D2" s="1">
+        <v>15</v>
+      </c>
+      <c r="D2" s="7">
         <f>5000/C2</f>
-        <v>357.14285714285717</v>
+        <v>333.33333333333331</v>
       </c>
       <c r="E2">
         <f>9.9/($B$10-1)</f>
         <v>0.1</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="6">
         <f>D2/$B$10</f>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="G2">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="G2" s="6">
         <f>(F2-1)*$B$12</f>
-        <v>12.831428571428573</v>
+        <v>11.643333333333333</v>
       </c>
       <c r="H2">
         <f>1024*$B$12*(F2-1)/$B$13</f>
-        <v>656.96914285714297</v>
+        <v>596.13866666666661</v>
       </c>
       <c r="I2">
         <f>_xlfn.FLOOR.MATH(H2)</f>
-        <v>656</v>
+        <v>596</v>
       </c>
       <c r="J2">
         <f>1+ ((I2/1024)*$B$13)/$B$12</f>
-        <v>3.5676352705410821</v>
+        <v>3.3327905811623246</v>
       </c>
       <c r="K2" s="4">
         <f>(F2-J2)/F2</f>
-        <v>1.0621242484970671E-3</v>
+        <v>1.6282565130252281E-4</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>250</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>3.25</v>
+        <v>2.35</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C7" si="0">B3*5</f>
-        <v>16.25</v>
-      </c>
-      <c r="D3" s="1">
-        <f t="shared" ref="D3:D7" si="1">5000/C3</f>
-        <v>307.69230769230768</v>
+        <f>B3*5</f>
+        <v>11.75</v>
+      </c>
+      <c r="D3" s="7">
+        <f>5000/C3</f>
+        <v>425.531914893617</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E8" si="2">9.9/($B$10-1)</f>
+        <f>9.9/($B$10-1)</f>
         <v>0.1</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F7" si="3">D3/$B$10</f>
-        <v>3.0769230769230766</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G7" si="4">(F3-1)*$B$12</f>
-        <v>10.363846153846152</v>
+      <c r="F3" s="6">
+        <f>D3/$B$10</f>
+        <v>4.2553191489361701</v>
+      </c>
+      <c r="G3" s="6">
+        <f>(F3-1)*$B$12</f>
+        <v>16.244042553191491</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H7" si="5">1024*$B$12*(F3-1)/$B$13</f>
-        <v>530.628923076923</v>
+        <f>1024*$B$12*(F3-1)/$B$13</f>
+        <v>831.69497872340435</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I7" si="6">_xlfn.FLOOR.MATH(H3)</f>
-        <v>530</v>
+        <f>_xlfn.FLOOR.MATH(H3)</f>
+        <v>831</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J7" si="7">1+ ((I3/1024)*$B$13)/$B$12</f>
-        <v>3.0744614228456912</v>
+        <f>1+ ((I3/1024)*$B$13)/$B$12</f>
+        <v>4.2525989478957911</v>
       </c>
       <c r="K3" s="4">
-        <f t="shared" ref="K3:K7" si="8">(F3-J3)/F3</f>
-        <v>8.0003757515025866E-4</v>
+        <f>(F3-J3)/F3</f>
+        <v>6.3924724448908069E-4</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>0.15</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="D4" s="1">
-        <f t="shared" si="1"/>
-        <v>333.33333333333331</v>
+        <f>B4*5</f>
+        <v>13.5</v>
+      </c>
+      <c r="D4" s="7">
+        <f>5000/C4</f>
+        <v>370.37037037037038</v>
       </c>
       <c r="E4">
-        <f t="shared" si="2"/>
+        <f>9.9/($B$10-1)</f>
         <v>0.1</v>
       </c>
-      <c r="F4">
-        <f t="shared" si="3"/>
-        <v>3.333333333333333</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="4"/>
-        <v>11.643333333333333</v>
+      <c r="F4" s="6">
+        <f>D4/$B$10</f>
+        <v>3.7037037037037037</v>
+      </c>
+      <c r="G4" s="6">
+        <f>(F4-1)*$B$12</f>
+        <v>13.491481481481483</v>
       </c>
       <c r="H4">
-        <f t="shared" si="5"/>
-        <v>596.13866666666661</v>
+        <f>1024*$B$12*(F4-1)/$B$13</f>
+        <v>690.76385185185188</v>
       </c>
       <c r="I4">
-        <f t="shared" si="6"/>
-        <v>596</v>
+        <f>_xlfn.FLOOR.MATH(H4)</f>
+        <v>690</v>
       </c>
       <c r="J4">
-        <f t="shared" si="7"/>
-        <v>3.3327905811623246</v>
+        <f>1+ ((I4/1024)*$B$13)/$B$12</f>
+        <v>3.7007139278557113</v>
       </c>
       <c r="K4" s="4">
-        <f t="shared" si="8"/>
-        <v>1.6282565130252281E-4</v>
+        <f>(F4-J4)/F4</f>
+        <v>8.0723947895795507E-4</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="0"/>
-        <v>13.5</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" si="1"/>
-        <v>370.37037037037038</v>
+        <f>B5*5</f>
+        <v>15</v>
+      </c>
+      <c r="D5" s="7">
+        <f>5000/C5</f>
+        <v>333.33333333333331</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
+        <f>9.9/($B$10-1)</f>
         <v>0.1</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="3"/>
-        <v>3.7037037037037037</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="4"/>
-        <v>13.491481481481483</v>
+      <c r="F5" s="6">
+        <f>D5/$B$10</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="G5" s="6">
+        <f>(F5-1)*$B$12</f>
+        <v>11.643333333333333</v>
       </c>
       <c r="H5">
-        <f t="shared" si="5"/>
-        <v>690.76385185185188</v>
+        <f>1024*$B$12*(F5-1)/$B$13</f>
+        <v>596.13866666666661</v>
       </c>
       <c r="I5">
-        <f t="shared" si="6"/>
-        <v>690</v>
+        <f>_xlfn.FLOOR.MATH(H5)</f>
+        <v>596</v>
       </c>
       <c r="J5">
-        <f t="shared" si="7"/>
-        <v>3.7007139278557113</v>
+        <f>1+ ((I5/1024)*$B$13)/$B$12</f>
+        <v>3.3327905811623246</v>
       </c>
       <c r="K5" s="4">
-        <f t="shared" si="8"/>
-        <v>8.0723947895795507E-4</v>
+        <f>(F5-J5)/F5</f>
+        <v>1.6282565130252281E-4</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>2</v>
+        <v>250</v>
       </c>
       <c r="B6" s="1">
-        <v>2.35</v>
+        <v>3.25</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="0"/>
-        <v>11.75</v>
-      </c>
-      <c r="D6" s="1">
-        <f t="shared" si="1"/>
-        <v>425.531914893617</v>
+        <f>B6*5</f>
+        <v>16.25</v>
+      </c>
+      <c r="D6" s="7">
+        <f>5000/C6</f>
+        <v>307.69230769230768</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
+        <f>9.9/($B$10-1)</f>
         <v>0.1</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="3"/>
-        <v>4.2553191489361701</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="4"/>
-        <v>16.244042553191491</v>
+      <c r="F6" s="6">
+        <f>D6/$B$10</f>
+        <v>3.0769230769230766</v>
+      </c>
+      <c r="G6" s="6">
+        <f>(F6-1)*$B$12</f>
+        <v>10.363846153846152</v>
       </c>
       <c r="H6">
-        <f t="shared" si="5"/>
-        <v>831.69497872340435</v>
+        <f>1024*$B$12*(F6-1)/$B$13</f>
+        <v>530.628923076923</v>
       </c>
       <c r="I6">
-        <f t="shared" si="6"/>
-        <v>831</v>
+        <f>_xlfn.FLOOR.MATH(H6)</f>
+        <v>530</v>
       </c>
       <c r="J6">
-        <f t="shared" si="7"/>
-        <v>4.2525989478957911</v>
+        <f>1+ ((I6/1024)*$B$13)/$B$12</f>
+        <v>3.0744614228456912</v>
       </c>
       <c r="K6" s="4">
-        <f t="shared" si="8"/>
-        <v>6.3924724448908069E-4</v>
+        <f>(F6-J6)/F6</f>
+        <v>8.0003757515025866E-4</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>45</v>
+        <v>3000</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="D7" s="1">
-        <f t="shared" si="1"/>
-        <v>333.33333333333331</v>
+        <f>B7*5</f>
+        <v>14</v>
+      </c>
+      <c r="D7" s="7">
+        <f>5000/C7</f>
+        <v>357.14285714285717</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
+        <f>9.9/($B$10-1)</f>
         <v>0.1</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="3"/>
-        <v>3.333333333333333</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="4"/>
-        <v>11.643333333333333</v>
+      <c r="F7" s="6">
+        <f>D7/$B$10</f>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="G7" s="6">
+        <f>(F7-1)*$B$12</f>
+        <v>12.831428571428573</v>
       </c>
       <c r="H7">
-        <f t="shared" si="5"/>
-        <v>596.13866666666661</v>
+        <f>1024*$B$12*(F7-1)/$B$13</f>
+        <v>656.96914285714297</v>
       </c>
       <c r="I7">
-        <f t="shared" si="6"/>
-        <v>596</v>
+        <f>_xlfn.FLOOR.MATH(H7)</f>
+        <v>656</v>
       </c>
       <c r="J7">
-        <f t="shared" si="7"/>
-        <v>3.3327905811623246</v>
+        <f>1+ ((I7/1024)*$B$13)/$B$12</f>
+        <v>3.5676352705410821</v>
       </c>
       <c r="K7" s="4">
-        <f t="shared" si="8"/>
-        <v>1.6282565130252281E-4</v>
+        <f>(F7-J7)/F7</f>
+        <v>1.0621242484970671E-3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C8" s="1">
+        <f>AVERAGE(C2:C7)</f>
+        <v>14.25</v>
+      </c>
       <c r="D8" s="3">
         <f>AVERAGE(D2:D7)</f>
-        <v>354.56735279430319</v>
+        <v>354.56735279430313</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E3:E8" si="0">9.9/($B$10-1)</f>
         <v>0.1</v>
       </c>
     </row>
@@ -897,6 +905,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K7">
+    <sortCondition ref="A2:A7"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -905,7 +916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D73221-315D-4403-8AB8-0BEE10775D1A}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>

</xml_diff>